<commit_message>
Create Country random name ve code eklendi
</commit_message>
<xml_diff>
--- a/src/main/resources/ScenarioResults.xlsx
+++ b/src/main/resources/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>login-functionality;login-with-valid-username-and-password</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>2020-12-12 12_05_48</t>
+  </si>
+  <si>
+    <t>country-functionality;create-country</t>
+  </si>
+  <si>
+    <t>2020-12-28 21_11_50</t>
   </si>
 </sst>
 </file>
@@ -95,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -199,6 +205,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>